<commit_message>
New term project rubric and draft lab 5 rubric
</commit_message>
<xml_diff>
--- a/Labs/Lab05-AI-Coding/CS210_Lab05_Rubric.xlsx
+++ b/Labs/Lab05-AI-Coding/CS210_Lab05_Rubric.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11122"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repos\CS210-Repos\CS210-CourseMaterials\Labs\Lab05-AI-Coding\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/DataCard/Repos/CS210-Repos/CS210-CourseMaterials/Labs/Lab05-AI-Coding/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D0EAC243-77C7-4BE6-A918-FE41A6DD8C3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{69F58E01-E5CD-3049-8681-60A5579FF52C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17172" yWindow="12" windowWidth="13572" windowHeight="16644" activeTab="1" xr2:uid="{5D75B731-65CD-014E-8BBA-DE69945DF98D}"/>
+    <workbookView xWindow="0" yWindow="540" windowWidth="26240" windowHeight="15500" activeTab="1" xr2:uid="{5D75B731-65CD-014E-8BBA-DE69945DF98D}"/>
   </bookViews>
   <sheets>
     <sheet name="Rubric" sheetId="1" r:id="rId1"/>
@@ -289,7 +289,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>1356360</xdr:colOff>
+          <xdr:colOff>1358900</xdr:colOff>
           <xdr:row>20</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
@@ -323,7 +323,7 @@
             </a:ln>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="32004" rIns="36576" bIns="32004" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="27432" bIns="22860" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="ctr" rtl="0">
@@ -334,8 +334,8 @@
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
-                  <a:latin typeface="Calibri"/>
-                  <a:cs typeface="Calibri"/>
+                  <a:latin typeface="Calibri" pitchFamily="2" charset="0"/>
+                  <a:cs typeface="Calibri" pitchFamily="2" charset="0"/>
                 </a:rPr>
                 <a:t>Reset</a:t>
               </a:r>
@@ -352,15 +352,15 @@
       <xdr:twoCellAnchor>
         <xdr:from>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>137160</xdr:colOff>
+          <xdr:colOff>139700</xdr:colOff>
           <xdr:row>20</xdr:row>
           <xdr:rowOff>190500</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>1356360</xdr:colOff>
+          <xdr:colOff>1358900</xdr:colOff>
           <xdr:row>22</xdr:row>
-          <xdr:rowOff>22860</xdr:rowOff>
+          <xdr:rowOff>25400</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -392,7 +392,7 @@
             </a:ln>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="32004" rIns="36576" bIns="32004" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="27432" bIns="22860" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="ctr" rtl="0">
@@ -403,8 +403,8 @@
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
-                  <a:latin typeface="Calibri"/>
-                  <a:cs typeface="Calibri"/>
+                  <a:latin typeface="Calibri" pitchFamily="2" charset="0"/>
+                  <a:cs typeface="Calibri" pitchFamily="2" charset="0"/>
                 </a:rPr>
                 <a:t>Add Comment</a:t>
               </a:r>
@@ -723,21 +723,21 @@
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="30.296875" customWidth="1"/>
+    <col min="1" max="1" width="30.33203125" customWidth="1"/>
     <col min="2" max="2" width="6" customWidth="1"/>
     <col min="3" max="3" width="38" customWidth="1"/>
-    <col min="4" max="4" width="7.296875" customWidth="1"/>
+    <col min="4" max="4" width="7.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>15</v>
       </c>
       <c r="E1" s="4"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="11" t="s">
         <v>14</v>
       </c>
@@ -746,14 +746,14 @@
       <c r="D2" s="12"/>
       <c r="E2" s="12"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="13"/>
       <c r="B3" s="13"/>
       <c r="C3" s="13"/>
       <c r="D3" s="13"/>
       <c r="E3" s="13"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="14" t="s">
         <v>1</v>
       </c>
@@ -762,7 +762,7 @@
       <c r="D4" s="14"/>
       <c r="E4" s="14"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="9" t="s">
         <v>3</v>
       </c>
@@ -773,7 +773,7 @@
       <c r="D5" s="2"/>
       <c r="E5" s="5"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -783,7 +783,7 @@
       <c r="D6" s="4"/>
       <c r="E6" s="8"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>16</v>
       </c>
@@ -792,7 +792,7 @@
       </c>
       <c r="E7" s="8"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>17</v>
       </c>
@@ -801,7 +801,7 @@
       </c>
       <c r="E8" s="8"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>18</v>
       </c>
@@ -810,7 +810,7 @@
       </c>
       <c r="E9" s="8"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>23</v>
       </c>
@@ -819,7 +819,7 @@
       </c>
       <c r="E10" s="8"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>19</v>
       </c>
@@ -828,7 +828,7 @@
       </c>
       <c r="E11" s="8"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -837,7 +837,7 @@
       </c>
       <c r="E12" s="8"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>20</v>
       </c>
@@ -846,7 +846,7 @@
       </c>
       <c r="E13" s="8"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>21</v>
       </c>
@@ -855,7 +855,7 @@
       </c>
       <c r="E14" s="8"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>22</v>
       </c>
@@ -864,10 +864,10 @@
       </c>
       <c r="E15" s="8"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E16" s="4"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="6" t="s">
         <v>5</v>
       </c>
@@ -878,7 +878,7 @@
       <c r="C17" s="6"/>
       <c r="E17" s="4"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E18" s="4"/>
     </row>
   </sheetData>
@@ -903,22 +903,22 @@
       <selection activeCell="A3" sqref="A3:E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="38" customWidth="1"/>
     <col min="2" max="2" width="8" customWidth="1"/>
-    <col min="3" max="3" width="5.69921875" customWidth="1"/>
+    <col min="3" max="3" width="5.6640625" customWidth="1"/>
     <col min="4" max="4" width="1" customWidth="1"/>
     <col min="5" max="5" width="27.5" style="4" customWidth="1"/>
-    <col min="6" max="6" width="11.19921875" customWidth="1"/>
+    <col min="6" max="6" width="11.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="20.55" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="20.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="11" t="s">
         <v>9</v>
       </c>
@@ -927,14 +927,14 @@
       <c r="D2" s="12"/>
       <c r="E2" s="12"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="13"/>
       <c r="B3" s="13"/>
       <c r="C3" s="13"/>
       <c r="D3" s="13"/>
       <c r="E3" s="13"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="14" t="s">
         <v>1</v>
       </c>
@@ -943,7 +943,7 @@
       <c r="D4" s="14"/>
       <c r="E4" s="14"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="9" t="s">
         <v>3</v>
       </c>
@@ -958,7 +958,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:6" s="3" customFormat="1" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" s="3" customFormat="1" ht="17.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -976,7 +976,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>16</v>
       </c>
@@ -993,7 +993,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>17</v>
       </c>
@@ -1010,7 +1010,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>18</v>
       </c>
@@ -1027,7 +1027,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>23</v>
       </c>
@@ -1044,7 +1044,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>19</v>
       </c>
@@ -1061,7 +1061,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -1078,7 +1078,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" s="3" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>20</v>
       </c>
@@ -1096,7 +1096,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" s="3" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>21</v>
       </c>
@@ -1114,7 +1114,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>22</v>
       </c>
@@ -1131,8 +1131,8 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="17" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="17" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
         <v>5</v>
       </c>
@@ -1145,41 +1145,41 @@
         <v>50</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B21" s="1"/>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B22" s="1"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="1"/>
     </row>
   </sheetData>
@@ -1202,15 +1202,15 @@
                 <anchor moveWithCells="1" sizeWithCells="1">
                   <from>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>137160</xdr:colOff>
+                    <xdr:colOff>139700</xdr:colOff>
                     <xdr:row>20</xdr:row>
                     <xdr:rowOff>190500</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>1356360</xdr:colOff>
+                    <xdr:colOff>1358900</xdr:colOff>
                     <xdr:row>22</xdr:row>
-                    <xdr:rowOff>22860</xdr:rowOff>
+                    <xdr:rowOff>25400</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -1230,7 +1230,7 @@
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>1356360</xdr:colOff>
+                    <xdr:colOff>1358900</xdr:colOff>
                     <xdr:row>20</xdr:row>
                     <xdr:rowOff>0</xdr:rowOff>
                   </to>

</xml_diff>